<commit_message>
Update GPS-RCB-M9N_rev.1.0_BOM 2025-04-23 22-22.xlsx
</commit_message>
<xml_diff>
--- a/Time-Card ТЕНШ.467883.001/ГНСС МОДУЛИ/UBlox/ТЕНШ.468157.01 RCB-NEO-M9N/Altium/ECAD/V1/Project Outputs for GPS-RCB-M9N/GPS-RCB-M9N_rev.1.0_BOM 2025-04-23 22-22.xlsx
+++ b/Time-Card ТЕНШ.467883.001/ГНСС МОДУЛИ/UBlox/ТЕНШ.468157.01 RCB-NEO-M9N/Altium/ECAD/V1/Project Outputs for GPS-RCB-M9N/GPS-RCB-M9N_rev.1.0_BOM 2025-04-23 22-22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Altium\SM_Project\QUANTUM\Time-Card ТЕНШ.467883.001\ГНСС МОДУЛИ\UBlox\ТЕНШ.468157.01 RCB-NEO-M9N\Altium\ECAD\V1\Project Outputs for GPS-RCB-M9N\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIWA\Documents\GitHub\QUANTUM\Time-Card ТЕНШ.467883.001\ГНСС МОДУЛИ\UBlox\ТЕНШ.468157.01 RCB-NEO-M9N\Altium\ECAD\V1\Project Outputs for GPS-RCB-M9N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A72AD1C4-EFA3-46F9-BA2C-698281A35C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC93F4B5-7737-40C0-BA1C-A4BAC5895F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1008" yWindow="1926" windowWidth="17280" windowHeight="9984" xr2:uid="{CBB020B5-8A20-49E0-B0BD-3B9A48A3DAD8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CBB020B5-8A20-49E0-B0BD-3B9A48A3DAD8}"/>
   </bookViews>
   <sheets>
     <sheet name="GPS-RCB-M9N_rev.1.0_BOM 2025-04" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>Designator</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Rf Coaxial Board Mount Connector</t>
   </si>
   <si>
-    <t>CONN_131-3711-301</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -238,13 +235,19 @@
   </si>
   <si>
     <t>IC NEO-M9N-00B</t>
+  </si>
+  <si>
+    <t>CONN_142-0711-301</t>
+  </si>
+  <si>
+    <t>CONN_142-0711-302</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,8 +256,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +274,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,12 +311,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -617,18 +636,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE519B57-FD9C-4771-972A-0E1C4B102764}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="18.26171875" customWidth="1"/>
-    <col min="5" max="5" width="27.83984375" customWidth="1"/>
-    <col min="6" max="6" width="9.26171875" customWidth="1"/>
-    <col min="7" max="7" width="27.1015625" customWidth="1"/>
-    <col min="8" max="8" width="15.3125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -654,7 +678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -676,7 +700,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -698,7 +722,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -720,7 +744,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -742,7 +766,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -764,43 +788,43 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -808,21 +832,21 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
@@ -830,21 +854,21 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -852,21 +876,21 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F11" s="1">
         <v>4</v>
@@ -874,21 +898,21 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
@@ -896,21 +920,21 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -918,21 +942,21 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
@@ -940,21 +964,21 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -963,6 +987,7 @@
       <c r="H15" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>